<commit_message>
Update master server history_v1.xlsx
</commit_message>
<xml_diff>
--- a/docs/master server history_v1.xlsx
+++ b/docs/master server history_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\reference\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CBC64FB-1E40-4580-ABB9-4A712879FC45}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF9DC61-271D-4247-977F-CAAFE7D4B659}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5880" yWindow="396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>계정명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,6 +36,257 @@
   </si>
   <si>
     <t>결과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>root</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>uname -sr</t>
+  </si>
+  <si>
+    <t>cat /etc/redhat-release</t>
+  </si>
+  <si>
+    <t>CentOS Linux release 7.3.1611 (Core)</t>
+  </si>
+  <si>
+    <t>Linux 3.10.0-514.2.2.el7.x86_64</t>
+  </si>
+  <si>
+    <t>cat /etc/hosts</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>127.0.0.1   localhost localhost.localdomain localhost4 localhost4.localdomain4
+::1         localhost localhost.localdomain localhost6 localhost6.localdomain6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setenforce 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setenforce: SELinux is disabled</t>
+  </si>
+  <si>
+    <t>sed -i --follow-symlinks 's/SELINUX=enforcing/SELINUX=disabled/g' /etc/sysconfig/selinux</t>
+  </si>
+  <si>
+    <t>목적</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>version check</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>disable selinux</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modprobe br_netfilter</t>
+  </si>
+  <si>
+    <t>echo '1' &gt; /proc/sys/net/bridge/bridge-nf-call-iptables</t>
+  </si>
+  <si>
+    <t>Enable br_netfilter Kernel Module</t>
+  </si>
+  <si>
+    <t>ll /proc/sys/net/</t>
+  </si>
+  <si>
+    <t>modprobe의 결과로 bridge 모듈 추가 확인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vi /etc/fstab</t>
+  </si>
+  <si>
+    <t>swapoff -a</t>
+  </si>
+  <si>
+    <t>추가 작업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>disable swap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>swap 줄의 앞에 #으로 주석처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yum install -y yum-utils device-mapper-persistent-data lvm2</t>
+  </si>
+  <si>
+    <t>install docker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yum install -y docker-ce</t>
+  </si>
+  <si>
+    <t>yum-config-manager --add-repo https://download.docker.com/linux/centos/docker-ce.repo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[kubernetes]
+name=Kubernetes
+baseurl=https://packages.cloud.google.com/yum/repos/kubernetes-el7-x86_64
+enabled=1
+gpgcheck=1
+repo_gpgcheck=1
+gpgkey=https://packages.cloud.google.com/yum/doc/yum-key.gpg https://packages.cloud.google.com/yum/doc/rpm-package-key.gpg
+EOF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cat &lt;&lt;EOF &gt; /etc/yum.repos.d/kubernetes.repo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yum install -y kubeadm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>install kubernetes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Updated:
+  device-mapper-persistent-data.x86_64 0:0.7.3-3.el7    lvm2.x86_64 7:2.02.180-10.el7_6.8    yum-utils.noarch 0:1.1.31-50.el7
+Dependency Updated:
+  device-mapper.x86_64 7:1.02.149-10.el7_6.8                        device-mapper-event.x86_64 7:1.02.149-10.el7_6.8
+  device-mapper-event-libs.x86_64 7:1.02.149-10.el7_6.8             device-mapper-libs.x86_64 7:1.02.149-10.el7_6.8
+  lvm2-libs.x86_64 7:2.02.180-10.el7_6.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Installed:
+  docker-ce.x86_64 3:18.09.7-3.el7
+Dependency Installed:
+  audit-libs-python.x86_64 0:2.8.4-4.el7  checkpolicy.x86_64 0:2.5-8.el7          container-selinux.noarch 2:2.99-1.el7_6
+  containerd.io.x86_64 0:1.2.6-3.3.el7    docker-ce-cli.x86_64 1:18.09.7-3.el7    libcgroup.x86_64 0:0.41-20.el7
+  libseccomp.x86_64 0:2.3.1-3.el7         libsemanage-python.x86_64 0:2.5-14.el7  policycoreutils-python.x86_64 0:2.5-29.el7_6.1
+  python-IPy.noarch 0:0.75-6.el7          setools-libs.x86_64 0:3.3.8-4.el7
+Dependency Updated:
+  audit.x86_64 0:2.8.4-4.el7                                 audit-libs.x86_64 0:2.8.4-4.el7
+  libselinux.x86_64 0:2.5-14.1.el7                           libselinux-python.x86_64 0:2.5-14.1.el7
+  libselinux-utils.x86_64 0:2.5-14.1.el7                     libsemanage.x86_64 0:2.5-14.el7
+  libsepol.x86_64 0:2.5-10.el7                               policycoreutils.x86_64 0:2.5-29.el7_6.1
+  selinux-policy.noarch 0:3.13.1-229.el7_6.12                selinux-policy-targeted.noarch 0:3.13.1-229.el7_6.12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Installed:
+  kubeadm.x86_64 0:1.15.0-0
+Dependency Installed:
+  conntrack-tools.x86_64 0:1.4.4-4.el7                            cri-tools.x86_64 0:1.13.0-0
+  kubectl.x86_64 0:1.15.0-0                                       kubelet.x86_64 0:1.15.0-0
+  kubernetes-cni.x86_64 0:0.7.5-0                                 libnetfilter_cthelper.x86_64 0:1.0.0-9.el7
+  libnetfilter_cttimeout.x86_64 0:1.0.0-6.el7                     libnetfilter_queue.x86_64 0:1.0.2-2.el7_2
+  socat.x86_64 0:1.7.3.2-2.el7
+Dependency Updated:
+  libnetfilter_conntrack.x86_64 0:1.0.6-1.el7_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">systemctl start kubelet &amp;&amp; systemctl enable kubelet </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>systemctl start docker &amp;&amp; systemctl enable docker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created symlink from /etc/systemd/system/multi-user.target.wants/docker.service to /usr/lib/systemd/system/docker.service.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Created symlink from /etc/systemd/system/multi-user.target.wants/kubelet.service to /usr/lib/systemd/system/kubelet.service.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Change the cgroup-driver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cgroup Driver: cgroupfs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>docker info | grep -i cgroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yum -y install etcd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>install etcd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Installed:
+  etcd.x86_64 0:3.3.11-2.el7.centos</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># [member]
+ETCD_LISTEN_PEER_URLS="http://192.168.99.100:2380"
+ETCD_LISTEN_CLIENT_URLS="http://192.168.99.100:2379"
+#[cluster]
+ETCD_INITIAL_ADVERTISE_PEER_URLS="http://192.168.99.100:2380"
+ETCD_INITIAL_CLUSTER="default=http://192.168.99.100:2380"
+ETCD_ADVERTISE_CLIENT_URLS="http://192.168.99.100:2379"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>systemctl start etcd</t>
+  </si>
+  <si>
+    <t>Created symlink from /etc/systemd/system/multi-user.target.wants/etcd.service to /usr/lib/systemd/system/etcd.service.</t>
+  </si>
+  <si>
+    <t>Job for etcd.service failed because the control process exited with error code. See "systemctl status etcd.service" and "journalctl -xe" for details.</t>
+  </si>
+  <si>
+    <t>vi /etc/etcd/etcd.conf</t>
+  </si>
+  <si>
+    <t>systemctl enable etcd</t>
+  </si>
+  <si>
+    <t>요약</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실패</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>configuratio etcd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>start etcd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yum -y install docker kubelet kubeadm kubectl kubernetes-cni flannel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Error: docker-ce conflicts with 2:docker-1.13.1-96.gitb2f74b2.el7.centos.x86_64
+Error: docker-ce-cli conflicts with 2:docker-1.13.1-96.gitb2f74b2.el7.centos.x86_64
+ You could try using --skip-broken to work around the problem
+** Found 2 pre-existing rpmdb problem(s), 'yum check' output follows:
+containerd.io-1.2.6-3.3.el7.x86_64 has installed conflicts containerd: containerd.io-1.2.6-3.3.el7.x86_64
+containerd.io-1.2.6-3.3.el7.x86_64 has installed conflicts runc: containerd.io-1.2.6-3.3.el7.x86_64</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -43,7 +294,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +304,21 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -79,8 +345,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -361,23 +639,286 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="41.69921875" defaultRowHeight="18.600000000000001" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="6.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="31" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="41.69921875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="18.600000000000001" customHeight="1">
+      <c r="B16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="18.600000000000001" customHeight="1">
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="18.600000000000001" customHeight="1">
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="18.600000000000001" customHeight="1">
+      <c r="B19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="18.600000000000001" customHeight="1">
+      <c r="B20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="18.600000000000001" customHeight="1">
+      <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="18.600000000000001" customHeight="1">
+      <c r="B22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="18.600000000000001" customHeight="1">
+      <c r="B23" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" ht="18.600000000000001" customHeight="1">
+      <c r="B24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="18.600000000000001" customHeight="1">
+      <c r="B25" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>